<commit_message>
medofmed error mod final
</commit_message>
<xml_diff>
--- a/Project1/Sorting data.xlsx
+++ b/Project1/Sorting data.xlsx
@@ -5,34 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seongminlee/Desktop/서울대학교/2019-2학기/고급프로그래밍방법론/Project1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seongminlee/Library/Containers/com.microsoft.Excel/Data/Desktop/서울대학교/2019-2학기/고급프로그래밍방법론/Project/Project1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59F19CD1-135E-AF43-AF57-FE4ACA45F665}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDEAF3C-42A0-4341-96F0-73A4030C1061}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="460" windowWidth="28300" windowHeight="16020" activeTab="2" xr2:uid="{9E2A00F2-D113-C34C-92E4-71E27140B445}"/>
+    <workbookView xWindow="440" yWindow="460" windowWidth="28300" windowHeight="16020" activeTab="1" xr2:uid="{9E2A00F2-D113-C34C-92E4-71E27140B445}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Summary" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet3!$A$2:$A$20</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet3!$B$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet3!$C$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet3!$C$2:$C$20</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet3!$D$1</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet3!$D$2:$D$20</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet3!$B$2:$B$20</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet3!$C$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet3!$C$2:$C$20</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet3!$D$1</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet3!$D$2:$D$20</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet3!$A$2:$A$20</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet3!$B$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet3!$B$2:$B$20</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -54,10 +38,6 @@
   </si>
   <si>
     <t>Insertion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Linear Quick</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -94,6 +74,10 @@
   </si>
   <si>
     <t>reverse initialize</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Med Quick</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -352,9 +336,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -372,18 +353,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
@@ -406,20 +375,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
@@ -432,6 +392,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -986,7 +970,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Linear Quick</c:v>
+                  <c:v>Med Quick</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1118,31 +1102,31 @@
                   <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.4</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.8</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.4</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.6</c:v>
+                  <c:v>8.6</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>10.8</c:v>
+                  <c:v>17.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>28</c:v>
+                  <c:v>47.6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>59.6</c:v>
+                  <c:v>95.8</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>122</c:v>
+                  <c:v>226</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3921,2372 +3905,2372 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F4AB8BF-51FF-9443-9B36-09D1976580E2}">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView topLeftCell="A68" workbookViewId="0">
+    <sheetView topLeftCell="A76" workbookViewId="0">
       <selection activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="17" t="s">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="17" t="s">
+      <c r="H1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="18" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="19">
+      <c r="A2" s="20">
         <v>10</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="7">
         <v>1</v>
       </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="20">
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="21"/>
-      <c r="B3" s="13">
+      <c r="B3" s="8">
         <v>2</v>
       </c>
-      <c r="C3" s="4">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0</v>
-      </c>
-      <c r="H3" s="22">
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="21"/>
-      <c r="B4" s="13">
+      <c r="B4" s="8">
         <v>3</v>
       </c>
-      <c r="C4" s="4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="22">
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="21"/>
-      <c r="B5" s="13">
+      <c r="B5" s="8">
         <v>4</v>
       </c>
-      <c r="C5" s="4">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0</v>
-      </c>
-      <c r="H5" s="22">
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="23"/>
-      <c r="B6" s="14">
+      <c r="A6" s="22"/>
+      <c r="B6" s="9">
         <v>5</v>
       </c>
-      <c r="C6" s="6">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="24">
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="19">
+      <c r="A7" s="20">
         <f>A2*10</f>
         <v>100</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="7">
         <v>1</v>
       </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0</v>
-      </c>
-      <c r="H7" s="20">
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="21"/>
-      <c r="B8" s="13">
+      <c r="B8" s="8">
         <v>2</v>
       </c>
-      <c r="C8" s="4">
-        <v>0</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0</v>
-      </c>
-      <c r="H8" s="22">
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="21"/>
-      <c r="B9" s="13">
+      <c r="B9" s="8">
         <v>3</v>
       </c>
-      <c r="C9" s="4">
-        <v>0</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0</v>
-      </c>
-      <c r="H9" s="22">
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="21"/>
-      <c r="B10" s="13">
+      <c r="B10" s="8">
         <v>4</v>
       </c>
-      <c r="C10" s="4">
-        <v>0</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0</v>
-      </c>
-      <c r="G10" s="4">
-        <v>0</v>
-      </c>
-      <c r="H10" s="22">
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="23"/>
-      <c r="B11" s="14">
+      <c r="A11" s="22"/>
+      <c r="B11" s="9">
         <v>5</v>
       </c>
-      <c r="C11" s="6">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0</v>
-      </c>
-      <c r="E11" s="6">
-        <v>0</v>
-      </c>
-      <c r="F11" s="6">
-        <v>0</v>
-      </c>
-      <c r="G11" s="6">
-        <v>0</v>
-      </c>
-      <c r="H11" s="24">
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0</v>
+      </c>
+      <c r="H11" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="19">
+      <c r="A12" s="20">
         <f>A7*10</f>
         <v>1000</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="7">
         <v>1</v>
       </c>
-      <c r="C12" s="2">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0</v>
-      </c>
-      <c r="H12" s="20">
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="21"/>
-      <c r="B13" s="13">
+      <c r="B13" s="8">
         <v>2</v>
       </c>
-      <c r="C13" s="4">
-        <v>0</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0</v>
-      </c>
-      <c r="E13" s="4">
-        <v>0</v>
-      </c>
-      <c r="F13" s="4">
-        <v>0</v>
-      </c>
-      <c r="G13" s="4">
-        <v>0</v>
-      </c>
-      <c r="H13" s="22">
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
+      <c r="H13" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="21"/>
-      <c r="B14" s="13">
+      <c r="B14" s="8">
         <v>3</v>
       </c>
-      <c r="C14" s="4">
-        <v>0</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0</v>
-      </c>
-      <c r="E14" s="4">
-        <v>0</v>
-      </c>
-      <c r="F14" s="4">
-        <v>0</v>
-      </c>
-      <c r="G14" s="4">
-        <v>0</v>
-      </c>
-      <c r="H14" s="22">
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="21"/>
-      <c r="B15" s="13">
+      <c r="B15" s="8">
         <v>4</v>
       </c>
-      <c r="C15" s="4">
-        <v>0</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0</v>
-      </c>
-      <c r="E15" s="4">
-        <v>0</v>
-      </c>
-      <c r="F15" s="4">
-        <v>0</v>
-      </c>
-      <c r="G15" s="4">
-        <v>0</v>
-      </c>
-      <c r="H15" s="22">
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="23"/>
-      <c r="B16" s="14">
+      <c r="A16" s="22"/>
+      <c r="B16" s="9">
         <v>5</v>
       </c>
-      <c r="C16" s="6">
-        <v>0</v>
-      </c>
-      <c r="D16" s="6">
-        <v>0</v>
-      </c>
-      <c r="E16" s="6">
-        <v>0</v>
-      </c>
-      <c r="F16" s="6">
-        <v>0</v>
-      </c>
-      <c r="G16" s="6">
-        <v>0</v>
-      </c>
-      <c r="H16" s="24">
+      <c r="C16" s="5">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0</v>
+      </c>
+      <c r="H16" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="19">
+      <c r="A17" s="20">
         <v>2000</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="7">
         <v>1</v>
       </c>
-      <c r="C17" s="2">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0</v>
-      </c>
-      <c r="G17" s="2">
-        <v>0</v>
-      </c>
-      <c r="H17" s="20">
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="14">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="21"/>
-      <c r="B18" s="13">
+      <c r="B18" s="8">
         <v>2</v>
       </c>
-      <c r="C18" s="4">
-        <v>0</v>
-      </c>
-      <c r="D18" s="4">
-        <v>0</v>
-      </c>
-      <c r="E18" s="4">
-        <v>0</v>
-      </c>
-      <c r="F18" s="4">
-        <v>0</v>
-      </c>
-      <c r="G18" s="4">
-        <v>0</v>
-      </c>
-      <c r="H18" s="22">
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+      <c r="H18" s="15">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="21"/>
-      <c r="B19" s="13">
+      <c r="B19" s="8">
         <v>3</v>
       </c>
-      <c r="C19" s="4">
-        <v>0</v>
-      </c>
-      <c r="D19" s="4">
-        <v>0</v>
-      </c>
-      <c r="E19" s="4">
-        <v>0</v>
-      </c>
-      <c r="F19" s="4">
-        <v>0</v>
-      </c>
-      <c r="G19" s="4">
-        <v>0</v>
-      </c>
-      <c r="H19" s="22">
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+      <c r="H19" s="15">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="21"/>
-      <c r="B20" s="13">
+      <c r="B20" s="8">
         <v>4</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>1</v>
       </c>
-      <c r="D20" s="4">
-        <v>0</v>
-      </c>
-      <c r="E20" s="4">
-        <v>0</v>
-      </c>
-      <c r="F20" s="4">
-        <v>0</v>
-      </c>
-      <c r="G20" s="4">
-        <v>0</v>
-      </c>
-      <c r="H20" s="22">
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0</v>
+      </c>
+      <c r="H20" s="15">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="23"/>
-      <c r="B21" s="14">
+      <c r="A21" s="22"/>
+      <c r="B21" s="9">
         <v>5</v>
       </c>
-      <c r="C21" s="6">
-        <v>0</v>
-      </c>
-      <c r="D21" s="6">
-        <v>0</v>
-      </c>
-      <c r="E21" s="6">
-        <v>0</v>
-      </c>
-      <c r="F21" s="6">
-        <v>0</v>
-      </c>
-      <c r="G21" s="6">
-        <v>0</v>
-      </c>
-      <c r="H21" s="24">
+      <c r="C21" s="5">
+        <v>0</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0</v>
+      </c>
+      <c r="H21" s="16">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="19">
+      <c r="A22" s="20">
         <v>5000</v>
       </c>
-      <c r="B22" s="12">
+      <c r="B22" s="7">
         <v>1</v>
       </c>
-      <c r="C22" s="2">
-        <v>0</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0</v>
-      </c>
-      <c r="F22" s="2">
-        <v>0</v>
-      </c>
-      <c r="G22" s="2">
-        <v>0</v>
-      </c>
-      <c r="H22" s="20">
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="14">
         <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="21"/>
-      <c r="B23" s="13">
+      <c r="B23" s="8">
         <v>2</v>
       </c>
-      <c r="C23" s="4">
-        <v>0</v>
-      </c>
-      <c r="D23" s="4">
-        <v>0</v>
-      </c>
-      <c r="E23" s="4">
-        <v>0</v>
-      </c>
-      <c r="F23" s="4">
-        <v>0</v>
-      </c>
-      <c r="G23" s="4">
-        <v>0</v>
-      </c>
-      <c r="H23" s="22">
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0</v>
+      </c>
+      <c r="H23" s="15">
         <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="21"/>
-      <c r="B24" s="13">
+      <c r="B24" s="8">
         <v>3</v>
       </c>
-      <c r="C24" s="4">
-        <v>0</v>
-      </c>
-      <c r="D24" s="4">
-        <v>0</v>
-      </c>
-      <c r="E24" s="4">
-        <v>0</v>
-      </c>
-      <c r="F24" s="4">
-        <v>0</v>
-      </c>
-      <c r="G24" s="4">
-        <v>0</v>
-      </c>
-      <c r="H24" s="22">
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0</v>
+      </c>
+      <c r="H24" s="15">
         <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="21"/>
-      <c r="B25" s="13">
+      <c r="B25" s="8">
         <v>4</v>
       </c>
-      <c r="C25" s="4">
-        <v>0</v>
-      </c>
-      <c r="D25" s="4">
-        <v>0</v>
-      </c>
-      <c r="E25" s="4">
-        <v>0</v>
-      </c>
-      <c r="F25" s="4">
-        <v>0</v>
-      </c>
-      <c r="G25" s="4">
-        <v>0</v>
-      </c>
-      <c r="H25" s="22">
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0</v>
+      </c>
+      <c r="H25" s="15">
         <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="23"/>
-      <c r="B26" s="14">
+      <c r="A26" s="22"/>
+      <c r="B26" s="9">
         <v>5</v>
       </c>
-      <c r="C26" s="6">
-        <v>0</v>
-      </c>
-      <c r="D26" s="6">
-        <v>0</v>
-      </c>
-      <c r="E26" s="6">
-        <v>0</v>
-      </c>
-      <c r="F26" s="6">
-        <v>0</v>
-      </c>
-      <c r="G26" s="6">
-        <v>0</v>
-      </c>
-      <c r="H26" s="24">
+      <c r="C26" s="5">
+        <v>0</v>
+      </c>
+      <c r="D26" s="5">
+        <v>0</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0</v>
+      </c>
+      <c r="H26" s="16">
         <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="19">
+      <c r="A27" s="20">
         <v>10000</v>
       </c>
-      <c r="B27" s="12">
+      <c r="B27" s="7">
         <v>1</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="1">
         <v>1</v>
       </c>
-      <c r="D27" s="2">
-        <v>0</v>
-      </c>
-      <c r="E27" s="2">
-        <v>0</v>
-      </c>
-      <c r="F27" s="2">
-        <v>0</v>
-      </c>
-      <c r="G27" s="2">
-        <v>0</v>
-      </c>
-      <c r="H27" s="20">
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
+      <c r="H27" s="14">
         <v>253</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="21"/>
-      <c r="B28" s="13">
+      <c r="B28" s="8">
         <v>2</v>
       </c>
-      <c r="C28" s="4">
-        <v>0</v>
-      </c>
-      <c r="D28" s="4">
-        <v>0</v>
-      </c>
-      <c r="E28" s="4">
-        <v>0</v>
-      </c>
-      <c r="F28" s="4">
-        <v>0</v>
-      </c>
-      <c r="G28" s="4">
-        <v>0</v>
-      </c>
-      <c r="H28" s="22">
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+      <c r="H28" s="15">
         <v>239</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="21"/>
-      <c r="B29" s="13">
+      <c r="B29" s="8">
         <v>3</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="3">
         <v>1</v>
       </c>
-      <c r="D29" s="4">
-        <v>0</v>
-      </c>
-      <c r="E29" s="4">
-        <v>0</v>
-      </c>
-      <c r="F29" s="4">
-        <v>0</v>
-      </c>
-      <c r="G29" s="4">
-        <v>0</v>
-      </c>
-      <c r="H29" s="22">
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0</v>
+      </c>
+      <c r="H29" s="15">
         <v>239</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="21"/>
-      <c r="B30" s="13">
+      <c r="B30" s="8">
         <v>4</v>
       </c>
-      <c r="C30" s="4">
-        <v>0</v>
-      </c>
-      <c r="D30" s="4">
-        <v>0</v>
-      </c>
-      <c r="E30" s="4">
-        <v>0</v>
-      </c>
-      <c r="F30" s="4">
-        <v>0</v>
-      </c>
-      <c r="G30" s="4">
-        <v>0</v>
-      </c>
-      <c r="H30" s="22">
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0</v>
+      </c>
+      <c r="H30" s="15">
         <v>239</v>
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="23"/>
-      <c r="B31" s="14">
+      <c r="A31" s="22"/>
+      <c r="B31" s="9">
         <v>5</v>
       </c>
-      <c r="C31" s="6">
-        <v>0</v>
-      </c>
-      <c r="D31" s="6">
-        <v>0</v>
-      </c>
-      <c r="E31" s="6">
-        <v>0</v>
-      </c>
-      <c r="F31" s="6">
-        <v>0</v>
-      </c>
-      <c r="G31" s="6">
-        <v>0</v>
-      </c>
-      <c r="H31" s="24">
+      <c r="C31" s="5">
+        <v>0</v>
+      </c>
+      <c r="D31" s="5">
+        <v>0</v>
+      </c>
+      <c r="E31" s="5">
+        <v>0</v>
+      </c>
+      <c r="F31" s="5">
+        <v>0</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0</v>
+      </c>
+      <c r="H31" s="16">
         <v>239</v>
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="19">
+      <c r="A32" s="20">
         <v>20000</v>
       </c>
-      <c r="B32" s="12">
+      <c r="B32" s="7">
         <v>1</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="1">
         <v>1</v>
       </c>
-      <c r="D32" s="2">
-        <v>0</v>
-      </c>
-      <c r="E32" s="2">
-        <v>0</v>
-      </c>
-      <c r="F32" s="2">
-        <v>0</v>
-      </c>
-      <c r="G32" s="2">
-        <v>0</v>
-      </c>
-      <c r="H32" s="20" t="s">
-        <v>8</v>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="21"/>
-      <c r="B33" s="13">
+      <c r="B33" s="8">
         <v>2</v>
       </c>
-      <c r="C33" s="4">
-        <v>0</v>
-      </c>
-      <c r="D33" s="4">
-        <v>0</v>
-      </c>
-      <c r="E33" s="4">
-        <v>0</v>
-      </c>
-      <c r="F33" s="4">
-        <v>0</v>
-      </c>
-      <c r="G33" s="4">
-        <v>0</v>
-      </c>
-      <c r="H33" s="22" t="s">
-        <v>8</v>
+      <c r="C33" s="3">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3">
+        <v>0</v>
+      </c>
+      <c r="G33" s="3">
+        <v>0</v>
+      </c>
+      <c r="H33" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="21"/>
-      <c r="B34" s="13">
+      <c r="B34" s="8">
         <v>3</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="3">
         <v>1</v>
       </c>
-      <c r="D34" s="4">
-        <v>0</v>
-      </c>
-      <c r="E34" s="4">
-        <v>0</v>
-      </c>
-      <c r="F34" s="4">
-        <v>0</v>
-      </c>
-      <c r="G34" s="4">
-        <v>0</v>
-      </c>
-      <c r="H34" s="22" t="s">
-        <v>8</v>
+      <c r="D34" s="3">
+        <v>0</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0</v>
+      </c>
+      <c r="G34" s="3">
+        <v>0</v>
+      </c>
+      <c r="H34" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="21"/>
-      <c r="B35" s="13">
+      <c r="B35" s="8">
         <v>4</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="3">
         <v>1</v>
       </c>
-      <c r="D35" s="4">
-        <v>0</v>
-      </c>
-      <c r="E35" s="4">
-        <v>0</v>
-      </c>
-      <c r="F35" s="4">
-        <v>0</v>
-      </c>
-      <c r="G35" s="4">
-        <v>0</v>
-      </c>
-      <c r="H35" s="22" t="s">
-        <v>8</v>
+      <c r="D35" s="3">
+        <v>0</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3">
+        <v>0</v>
+      </c>
+      <c r="G35" s="3">
+        <v>0</v>
+      </c>
+      <c r="H35" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="23"/>
-      <c r="B36" s="14">
+      <c r="A36" s="22"/>
+      <c r="B36" s="9">
         <v>5</v>
       </c>
-      <c r="C36" s="6">
-        <v>0</v>
-      </c>
-      <c r="D36" s="6">
-        <v>0</v>
-      </c>
-      <c r="E36" s="6">
-        <v>0</v>
-      </c>
-      <c r="F36" s="6">
-        <v>0</v>
-      </c>
-      <c r="G36" s="6">
-        <v>0</v>
-      </c>
-      <c r="H36" s="24" t="s">
-        <v>8</v>
+      <c r="C36" s="5">
+        <v>0</v>
+      </c>
+      <c r="D36" s="5">
+        <v>0</v>
+      </c>
+      <c r="E36" s="5">
+        <v>0</v>
+      </c>
+      <c r="F36" s="5">
+        <v>0</v>
+      </c>
+      <c r="G36" s="5">
+        <v>0</v>
+      </c>
+      <c r="H36" s="16" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="19">
+      <c r="A37" s="20">
         <v>50000</v>
       </c>
-      <c r="B37" s="12">
+      <c r="B37" s="7">
         <v>1</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="1">
         <v>4</v>
       </c>
-      <c r="D37" s="2">
-        <v>0</v>
-      </c>
-      <c r="E37" s="2">
-        <v>0</v>
-      </c>
-      <c r="F37" s="2">
-        <v>0</v>
-      </c>
-      <c r="G37" s="2">
-        <v>0</v>
-      </c>
-      <c r="H37" s="20" t="s">
-        <v>8</v>
+      <c r="D37" s="1">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0</v>
+      </c>
+      <c r="H37" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="21"/>
-      <c r="B38" s="13">
+      <c r="B38" s="8">
         <v>2</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="3">
         <v>4</v>
       </c>
-      <c r="D38" s="4">
-        <v>0</v>
-      </c>
-      <c r="E38" s="4">
-        <v>0</v>
-      </c>
-      <c r="F38" s="4">
-        <v>0</v>
-      </c>
-      <c r="G38" s="4">
-        <v>0</v>
-      </c>
-      <c r="H38" s="22" t="s">
-        <v>8</v>
+      <c r="D38" s="3">
+        <v>0</v>
+      </c>
+      <c r="E38" s="3">
+        <v>0</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0</v>
+      </c>
+      <c r="G38" s="3">
+        <v>0</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="21"/>
-      <c r="B39" s="13">
+      <c r="B39" s="8">
         <v>3</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="3">
         <v>4</v>
       </c>
-      <c r="D39" s="4">
-        <v>0</v>
-      </c>
-      <c r="E39" s="4">
-        <v>0</v>
-      </c>
-      <c r="F39" s="4">
-        <v>0</v>
-      </c>
-      <c r="G39" s="4">
-        <v>0</v>
-      </c>
-      <c r="H39" s="22" t="s">
-        <v>8</v>
+      <c r="D39" s="3">
+        <v>0</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0</v>
+      </c>
+      <c r="H39" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="21"/>
-      <c r="B40" s="13">
+      <c r="B40" s="8">
         <v>4</v>
       </c>
-      <c r="C40" s="4">
+      <c r="C40" s="3">
         <v>4</v>
       </c>
-      <c r="D40" s="4">
-        <v>0</v>
-      </c>
-      <c r="E40" s="4">
-        <v>0</v>
-      </c>
-      <c r="F40" s="4">
-        <v>0</v>
-      </c>
-      <c r="G40" s="4">
-        <v>0</v>
-      </c>
-      <c r="H40" s="22" t="s">
-        <v>8</v>
+      <c r="D40" s="3">
+        <v>0</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0</v>
+      </c>
+      <c r="G40" s="3">
+        <v>0</v>
+      </c>
+      <c r="H40" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="23"/>
-      <c r="B41" s="14">
+      <c r="A41" s="22"/>
+      <c r="B41" s="9">
         <v>5</v>
       </c>
-      <c r="C41" s="6">
+      <c r="C41" s="5">
         <v>4</v>
       </c>
-      <c r="D41" s="6">
-        <v>0</v>
-      </c>
-      <c r="E41" s="6">
-        <v>0</v>
-      </c>
-      <c r="F41" s="6">
-        <v>0</v>
-      </c>
-      <c r="G41" s="6">
-        <v>0</v>
-      </c>
-      <c r="H41" s="24" t="s">
-        <v>8</v>
+      <c r="D41" s="5">
+        <v>0</v>
+      </c>
+      <c r="E41" s="5">
+        <v>0</v>
+      </c>
+      <c r="F41" s="5">
+        <v>0</v>
+      </c>
+      <c r="G41" s="5">
+        <v>0</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="19">
+      <c r="A42" s="20">
         <v>100000</v>
       </c>
-      <c r="B42" s="12">
+      <c r="B42" s="7">
         <v>1</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="1">
         <v>17</v>
       </c>
-      <c r="D42" s="2">
-        <v>0</v>
-      </c>
-      <c r="E42" s="2">
-        <v>0</v>
-      </c>
-      <c r="F42" s="2">
-        <v>0</v>
-      </c>
-      <c r="G42" s="2">
-        <v>0</v>
-      </c>
-      <c r="H42" s="20" t="s">
-        <v>8</v>
+      <c r="D42" s="1">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0</v>
+      </c>
+      <c r="G42" s="1">
+        <v>0</v>
+      </c>
+      <c r="H42" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="21"/>
-      <c r="B43" s="13">
+      <c r="B43" s="8">
         <v>2</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43" s="3">
         <v>18</v>
       </c>
-      <c r="D43" s="4">
-        <v>0</v>
-      </c>
-      <c r="E43" s="4">
-        <v>0</v>
-      </c>
-      <c r="F43" s="4">
-        <v>0</v>
-      </c>
-      <c r="G43" s="4">
-        <v>0</v>
-      </c>
-      <c r="H43" s="22" t="s">
-        <v>8</v>
+      <c r="D43" s="3">
+        <v>0</v>
+      </c>
+      <c r="E43" s="3">
+        <v>0</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0</v>
+      </c>
+      <c r="G43" s="3">
+        <v>0</v>
+      </c>
+      <c r="H43" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="21"/>
-      <c r="B44" s="13">
+      <c r="B44" s="8">
         <v>3</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C44" s="3">
         <v>16</v>
       </c>
-      <c r="D44" s="4">
-        <v>0</v>
-      </c>
-      <c r="E44" s="4">
-        <v>0</v>
-      </c>
-      <c r="F44" s="4">
-        <v>0</v>
-      </c>
-      <c r="G44" s="4">
-        <v>0</v>
-      </c>
-      <c r="H44" s="22" t="s">
-        <v>8</v>
+      <c r="D44" s="3">
+        <v>0</v>
+      </c>
+      <c r="E44" s="3">
+        <v>0</v>
+      </c>
+      <c r="F44" s="3">
+        <v>0</v>
+      </c>
+      <c r="G44" s="3">
+        <v>0</v>
+      </c>
+      <c r="H44" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="21"/>
-      <c r="B45" s="13">
+      <c r="B45" s="8">
         <v>4</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C45" s="3">
         <v>17</v>
       </c>
-      <c r="D45" s="4">
-        <v>0</v>
-      </c>
-      <c r="E45" s="4">
-        <v>0</v>
-      </c>
-      <c r="F45" s="4">
-        <v>0</v>
-      </c>
-      <c r="G45" s="4">
-        <v>0</v>
-      </c>
-      <c r="H45" s="22" t="s">
-        <v>8</v>
+      <c r="D45" s="3">
+        <v>0</v>
+      </c>
+      <c r="E45" s="3">
+        <v>0</v>
+      </c>
+      <c r="F45" s="3">
+        <v>0</v>
+      </c>
+      <c r="G45" s="3">
+        <v>0</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="23"/>
-      <c r="B46" s="14">
+      <c r="A46" s="22"/>
+      <c r="B46" s="9">
         <v>5</v>
       </c>
-      <c r="C46" s="6">
+      <c r="C46" s="5">
         <v>15</v>
       </c>
-      <c r="D46" s="6">
-        <v>0</v>
-      </c>
-      <c r="E46" s="6">
-        <v>0</v>
-      </c>
-      <c r="F46" s="6">
-        <v>0</v>
-      </c>
-      <c r="G46" s="6">
-        <v>0</v>
-      </c>
-      <c r="H46" s="24" t="s">
-        <v>8</v>
+      <c r="D46" s="5">
+        <v>0</v>
+      </c>
+      <c r="E46" s="5">
+        <v>0</v>
+      </c>
+      <c r="F46" s="5">
+        <v>0</v>
+      </c>
+      <c r="G46" s="5">
+        <v>0</v>
+      </c>
+      <c r="H46" s="16" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="19">
+      <c r="A47" s="20">
         <v>200000</v>
       </c>
-      <c r="B47" s="12">
+      <c r="B47" s="7">
         <v>1</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="1">
         <v>59</v>
       </c>
-      <c r="D47" s="2">
-        <v>0</v>
-      </c>
-      <c r="E47" s="2">
-        <v>0</v>
-      </c>
-      <c r="F47" s="2">
-        <v>0</v>
-      </c>
-      <c r="G47" s="2">
-        <v>0</v>
-      </c>
-      <c r="H47" s="20" t="s">
-        <v>8</v>
+      <c r="D47" s="1">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0</v>
+      </c>
+      <c r="F47" s="1">
+        <v>0</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0</v>
+      </c>
+      <c r="H47" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="21"/>
-      <c r="B48" s="13">
+      <c r="B48" s="8">
         <v>2</v>
       </c>
-      <c r="C48" s="4">
+      <c r="C48" s="3">
         <v>58</v>
       </c>
-      <c r="D48" s="4">
-        <v>0</v>
-      </c>
-      <c r="E48" s="4">
-        <v>0</v>
-      </c>
-      <c r="F48" s="4">
-        <v>0</v>
-      </c>
-      <c r="G48" s="4">
-        <v>0</v>
-      </c>
-      <c r="H48" s="22" t="s">
-        <v>8</v>
+      <c r="D48" s="3">
+        <v>0</v>
+      </c>
+      <c r="E48" s="3">
+        <v>0</v>
+      </c>
+      <c r="F48" s="3">
+        <v>1</v>
+      </c>
+      <c r="G48" s="3">
+        <v>0</v>
+      </c>
+      <c r="H48" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="21"/>
-      <c r="B49" s="13">
+      <c r="B49" s="8">
         <v>3</v>
       </c>
-      <c r="C49" s="4">
+      <c r="C49" s="3">
         <v>63</v>
       </c>
-      <c r="D49" s="4">
-        <v>0</v>
-      </c>
-      <c r="E49" s="4">
-        <v>0</v>
-      </c>
-      <c r="F49" s="4">
-        <v>0</v>
-      </c>
-      <c r="G49" s="4">
-        <v>0</v>
-      </c>
-      <c r="H49" s="22" t="s">
-        <v>8</v>
+      <c r="D49" s="3">
+        <v>0</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0</v>
+      </c>
+      <c r="F49" s="3">
+        <v>0</v>
+      </c>
+      <c r="G49" s="3">
+        <v>0</v>
+      </c>
+      <c r="H49" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="21"/>
-      <c r="B50" s="13">
+      <c r="B50" s="8">
         <v>4</v>
       </c>
-      <c r="C50" s="4">
+      <c r="C50" s="3">
         <v>64</v>
       </c>
-      <c r="D50" s="4">
-        <v>0</v>
-      </c>
-      <c r="E50" s="4">
-        <v>0</v>
-      </c>
-      <c r="F50" s="4">
+      <c r="D50" s="3">
+        <v>0</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0</v>
+      </c>
+      <c r="G50" s="3">
+        <v>0</v>
+      </c>
+      <c r="H50" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="22"/>
+      <c r="B51" s="9">
+        <v>5</v>
+      </c>
+      <c r="C51" s="5">
+        <v>63</v>
+      </c>
+      <c r="D51" s="5">
+        <v>0</v>
+      </c>
+      <c r="E51" s="5">
         <v>1</v>
       </c>
-      <c r="G50" s="4">
-        <v>0</v>
-      </c>
-      <c r="H50" s="22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="23"/>
-      <c r="B51" s="14">
-        <v>5</v>
-      </c>
-      <c r="C51" s="6">
-        <v>63</v>
-      </c>
-      <c r="D51" s="6">
-        <v>0</v>
-      </c>
-      <c r="E51" s="6">
+      <c r="F51" s="5">
+        <v>0</v>
+      </c>
+      <c r="G51" s="5">
+        <v>0</v>
+      </c>
+      <c r="H51" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="20">
+        <v>500000</v>
+      </c>
+      <c r="B52" s="7">
         <v>1</v>
       </c>
-      <c r="F51" s="6">
-        <v>0</v>
-      </c>
-      <c r="G51" s="6">
-        <v>0</v>
-      </c>
-      <c r="H51" s="24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="19">
-        <v>500000</v>
-      </c>
-      <c r="B52" s="12">
+      <c r="C52" s="1">
+        <v>375</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <v>0</v>
+      </c>
+      <c r="G52" s="1">
         <v>1</v>
       </c>
-      <c r="C52" s="2">
-        <v>375</v>
-      </c>
-      <c r="D52" s="2">
-        <v>0</v>
-      </c>
-      <c r="E52" s="2">
-        <v>0</v>
-      </c>
-      <c r="F52" s="2">
-        <v>0</v>
-      </c>
-      <c r="G52" s="2">
-        <v>1</v>
-      </c>
-      <c r="H52" s="20" t="s">
-        <v>8</v>
+      <c r="H52" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="21"/>
-      <c r="B53" s="13">
+      <c r="B53" s="8">
         <v>2</v>
       </c>
-      <c r="C53" s="4">
+      <c r="C53" s="3">
         <v>365</v>
       </c>
-      <c r="D53" s="4">
-        <v>0</v>
-      </c>
-      <c r="E53" s="4">
-        <v>0</v>
-      </c>
-      <c r="F53" s="4">
-        <v>0</v>
-      </c>
-      <c r="G53" s="4">
-        <v>0</v>
-      </c>
-      <c r="H53" s="22" t="s">
-        <v>8</v>
+      <c r="D53" s="3">
+        <v>0</v>
+      </c>
+      <c r="E53" s="3">
+        <v>0</v>
+      </c>
+      <c r="F53" s="3">
+        <v>0</v>
+      </c>
+      <c r="G53" s="3">
+        <v>0</v>
+      </c>
+      <c r="H53" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="21"/>
-      <c r="B54" s="13">
+      <c r="B54" s="8">
         <v>3</v>
       </c>
-      <c r="C54" s="4">
+      <c r="C54" s="3">
         <v>381</v>
       </c>
-      <c r="D54" s="4">
-        <v>0</v>
-      </c>
-      <c r="E54" s="4">
-        <v>0</v>
-      </c>
-      <c r="F54" s="4">
-        <v>1</v>
-      </c>
-      <c r="G54" s="4">
-        <v>0</v>
-      </c>
-      <c r="H54" s="22" t="s">
-        <v>8</v>
+      <c r="D54" s="3">
+        <v>0</v>
+      </c>
+      <c r="E54" s="3">
+        <v>0</v>
+      </c>
+      <c r="F54" s="3">
+        <v>0</v>
+      </c>
+      <c r="G54" s="3">
+        <v>0</v>
+      </c>
+      <c r="H54" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="21"/>
-      <c r="B55" s="13">
+      <c r="B55" s="8">
         <v>4</v>
       </c>
-      <c r="C55" s="4">
+      <c r="C55" s="3">
         <v>404</v>
       </c>
-      <c r="D55" s="4">
-        <v>0</v>
-      </c>
-      <c r="E55" s="4">
-        <v>0</v>
-      </c>
-      <c r="F55" s="4">
+      <c r="D55" s="3">
+        <v>0</v>
+      </c>
+      <c r="E55" s="3">
+        <v>0</v>
+      </c>
+      <c r="F55" s="3">
         <v>1</v>
       </c>
-      <c r="G55" s="4">
-        <v>0</v>
-      </c>
-      <c r="H55" s="22" t="s">
-        <v>8</v>
+      <c r="G55" s="3">
+        <v>0</v>
+      </c>
+      <c r="H55" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="23"/>
-      <c r="B56" s="14">
+      <c r="A56" s="22"/>
+      <c r="B56" s="9">
         <v>5</v>
       </c>
-      <c r="C56" s="6">
+      <c r="C56" s="5">
         <v>377</v>
       </c>
-      <c r="D56" s="6">
-        <v>0</v>
-      </c>
-      <c r="E56" s="6">
-        <v>0</v>
-      </c>
-      <c r="F56" s="6">
-        <v>0</v>
-      </c>
-      <c r="G56" s="6">
-        <v>0</v>
-      </c>
-      <c r="H56" s="24" t="s">
-        <v>8</v>
+      <c r="D56" s="5">
+        <v>0</v>
+      </c>
+      <c r="E56" s="5">
+        <v>0</v>
+      </c>
+      <c r="F56" s="5">
+        <v>0</v>
+      </c>
+      <c r="G56" s="5">
+        <v>0</v>
+      </c>
+      <c r="H56" s="16" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="19">
+      <c r="A57" s="20">
         <v>1000000</v>
       </c>
-      <c r="B57" s="12">
+      <c r="B57" s="7">
         <v>1</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D57" s="2">
-        <v>0</v>
-      </c>
-      <c r="E57" s="2">
+      <c r="C57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1">
         <v>1</v>
       </c>
-      <c r="F57" s="2">
+      <c r="F57" s="1">
         <v>1</v>
       </c>
-      <c r="G57" s="2">
-        <v>0</v>
-      </c>
-      <c r="H57" s="20" t="s">
-        <v>8</v>
+      <c r="G57" s="1">
+        <v>0</v>
+      </c>
+      <c r="H57" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="21"/>
-      <c r="B58" s="13">
+      <c r="B58" s="8">
         <v>2</v>
       </c>
-      <c r="C58" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D58" s="4">
+      <c r="C58" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" s="3">
         <v>1</v>
       </c>
-      <c r="E58" s="4">
-        <v>0</v>
-      </c>
-      <c r="F58" s="4">
+      <c r="E58" s="3">
+        <v>0</v>
+      </c>
+      <c r="F58" s="3">
         <v>1</v>
       </c>
-      <c r="G58" s="4">
+      <c r="G58" s="3">
         <v>1</v>
       </c>
-      <c r="H58" s="22" t="s">
-        <v>8</v>
+      <c r="H58" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="21"/>
-      <c r="B59" s="13">
+      <c r="B59" s="8">
         <v>3</v>
       </c>
-      <c r="C59" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D59" s="4">
-        <v>0</v>
-      </c>
-      <c r="E59" s="4">
-        <v>0</v>
-      </c>
-      <c r="F59" s="4">
+      <c r="C59" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="3">
+        <v>0</v>
+      </c>
+      <c r="E59" s="3">
+        <v>0</v>
+      </c>
+      <c r="F59" s="3">
         <v>1</v>
       </c>
-      <c r="G59" s="4">
-        <v>0</v>
-      </c>
-      <c r="H59" s="22" t="s">
-        <v>8</v>
+      <c r="G59" s="3">
+        <v>0</v>
+      </c>
+      <c r="H59" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="21"/>
-      <c r="B60" s="13">
+      <c r="B60" s="8">
         <v>4</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D60" s="4">
-        <v>0</v>
-      </c>
-      <c r="E60" s="4">
-        <v>0</v>
-      </c>
-      <c r="F60" s="4">
+      <c r="C60" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="3">
+        <v>0</v>
+      </c>
+      <c r="E60" s="3">
+        <v>0</v>
+      </c>
+      <c r="F60" s="3">
+        <v>0</v>
+      </c>
+      <c r="G60" s="3">
+        <v>0</v>
+      </c>
+      <c r="H60" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="22"/>
+      <c r="B61" s="9">
+        <v>5</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="5">
+        <v>0</v>
+      </c>
+      <c r="E61" s="5">
+        <v>0</v>
+      </c>
+      <c r="F61" s="5">
         <v>1</v>
       </c>
-      <c r="G60" s="4">
-        <v>0</v>
-      </c>
-      <c r="H60" s="22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
-      <c r="A61" s="23"/>
-      <c r="B61" s="14">
-        <v>5</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D61" s="6">
-        <v>0</v>
-      </c>
-      <c r="E61" s="6">
-        <v>0</v>
-      </c>
-      <c r="F61" s="6">
-        <v>0</v>
-      </c>
-      <c r="G61" s="6">
-        <v>0</v>
-      </c>
-      <c r="H61" s="24" t="s">
-        <v>8</v>
+      <c r="G61" s="5">
+        <v>0</v>
+      </c>
+      <c r="H61" s="16" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="19">
+      <c r="A62" s="20">
         <v>2000000</v>
       </c>
-      <c r="B62" s="12">
+      <c r="B62" s="7">
         <v>1</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D62" s="2">
-        <v>0</v>
-      </c>
-      <c r="E62" s="2">
-        <v>0</v>
-      </c>
-      <c r="F62" s="2">
+      <c r="C62" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" s="1">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1">
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <v>2</v>
+      </c>
+      <c r="G62" s="1">
         <v>1</v>
       </c>
-      <c r="G62" s="2">
-        <v>1</v>
-      </c>
-      <c r="H62" s="20" t="s">
-        <v>8</v>
+      <c r="H62" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="21"/>
-      <c r="B63" s="13">
+      <c r="B63" s="8">
         <v>2</v>
       </c>
-      <c r="C63" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D63" s="4">
+      <c r="C63" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="3">
         <v>1</v>
       </c>
-      <c r="E63" s="4">
+      <c r="E63" s="3">
         <v>1</v>
       </c>
-      <c r="F63" s="4">
-        <v>0</v>
-      </c>
-      <c r="G63" s="4">
+      <c r="F63" s="3">
+        <v>2</v>
+      </c>
+      <c r="G63" s="3">
         <v>1</v>
       </c>
-      <c r="H63" s="22" t="s">
-        <v>8</v>
+      <c r="H63" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="21"/>
-      <c r="B64" s="13">
+      <c r="B64" s="8">
         <v>3</v>
       </c>
-      <c r="C64" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D64" s="4">
-        <v>0</v>
-      </c>
-      <c r="E64" s="4">
+      <c r="C64" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" s="3">
+        <v>0</v>
+      </c>
+      <c r="E64" s="3">
         <v>1</v>
       </c>
-      <c r="F64" s="4">
+      <c r="F64" s="3">
         <v>1</v>
       </c>
-      <c r="G64" s="4">
+      <c r="G64" s="3">
         <v>1</v>
       </c>
-      <c r="H64" s="22" t="s">
-        <v>8</v>
+      <c r="H64" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="21"/>
-      <c r="B65" s="13">
+      <c r="B65" s="8">
         <v>4</v>
       </c>
-      <c r="C65" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D65" s="4">
-        <v>0</v>
-      </c>
-      <c r="E65" s="4">
-        <v>0</v>
-      </c>
-      <c r="F65" s="4">
+      <c r="C65" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" s="3">
+        <v>0</v>
+      </c>
+      <c r="E65" s="3">
+        <v>0</v>
+      </c>
+      <c r="F65" s="3">
+        <v>2</v>
+      </c>
+      <c r="G65" s="3">
+        <v>2</v>
+      </c>
+      <c r="H65" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="22"/>
+      <c r="B66" s="9">
+        <v>5</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" s="5">
+        <v>0</v>
+      </c>
+      <c r="E66" s="5">
+        <v>0</v>
+      </c>
+      <c r="F66" s="5">
+        <v>2</v>
+      </c>
+      <c r="G66" s="5">
         <v>1</v>
       </c>
-      <c r="G65" s="4">
-        <v>2</v>
-      </c>
-      <c r="H65" s="22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
-      <c r="A66" s="23"/>
-      <c r="B66" s="14">
-        <v>5</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D66" s="6">
-        <v>0</v>
-      </c>
-      <c r="E66" s="6">
-        <v>0</v>
-      </c>
-      <c r="F66" s="6">
+      <c r="H66" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="20">
+        <v>5000000</v>
+      </c>
+      <c r="B67" s="7">
         <v>1</v>
       </c>
-      <c r="G66" s="6">
+      <c r="C67" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" s="1">
         <v>1</v>
       </c>
-      <c r="H66" s="24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
-      <c r="A67" s="19">
-        <v>5000000</v>
-      </c>
-      <c r="B67" s="12">
+      <c r="E67" s="1">
         <v>1</v>
       </c>
-      <c r="C67" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D67" s="2">
-        <v>1</v>
-      </c>
-      <c r="E67" s="2">
-        <v>1</v>
-      </c>
-      <c r="F67" s="2">
-        <v>3</v>
-      </c>
-      <c r="G67" s="2">
+      <c r="F67" s="1">
         <v>4</v>
       </c>
-      <c r="H67" s="20" t="s">
-        <v>8</v>
+      <c r="G67" s="1">
+        <v>4</v>
+      </c>
+      <c r="H67" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="21"/>
-      <c r="B68" s="13">
+      <c r="B68" s="8">
         <v>2</v>
       </c>
-      <c r="C68" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D68" s="4">
+      <c r="C68" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="3">
         <v>1</v>
       </c>
-      <c r="E68" s="4">
+      <c r="E68" s="3">
         <v>1</v>
       </c>
-      <c r="F68" s="4">
-        <v>2</v>
-      </c>
-      <c r="G68" s="4">
+      <c r="F68" s="3">
+        <v>4</v>
+      </c>
+      <c r="G68" s="3">
         <v>3</v>
       </c>
-      <c r="H68" s="22" t="s">
-        <v>8</v>
+      <c r="H68" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="21"/>
-      <c r="B69" s="13">
+      <c r="B69" s="8">
         <v>3</v>
       </c>
-      <c r="C69" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D69" s="4">
+      <c r="C69" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" s="3">
         <v>1</v>
       </c>
-      <c r="E69" s="4">
+      <c r="E69" s="3">
         <v>1</v>
       </c>
-      <c r="F69" s="4">
-        <v>2</v>
-      </c>
-      <c r="G69" s="4">
+      <c r="F69" s="3">
+        <v>4</v>
+      </c>
+      <c r="G69" s="3">
         <v>3</v>
       </c>
-      <c r="H69" s="22" t="s">
-        <v>8</v>
+      <c r="H69" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" s="21"/>
-      <c r="B70" s="13">
+      <c r="B70" s="8">
         <v>4</v>
       </c>
-      <c r="C70" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D70" s="4">
+      <c r="C70" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" s="3">
         <v>1</v>
       </c>
-      <c r="E70" s="4">
+      <c r="E70" s="3">
         <v>1</v>
       </c>
-      <c r="F70" s="4">
+      <c r="F70" s="3">
+        <v>4</v>
+      </c>
+      <c r="G70" s="3">
         <v>3</v>
       </c>
-      <c r="G70" s="4">
+      <c r="H70" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="22"/>
+      <c r="B71" s="9">
+        <v>5</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" s="5">
+        <v>1</v>
+      </c>
+      <c r="E71" s="5">
+        <v>1</v>
+      </c>
+      <c r="F71" s="5">
+        <v>4</v>
+      </c>
+      <c r="G71" s="5">
         <v>3</v>
       </c>
-      <c r="H70" s="22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8">
-      <c r="A71" s="23"/>
-      <c r="B71" s="14">
-        <v>5</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D71" s="6">
+      <c r="H71" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="20">
+        <v>10000000</v>
+      </c>
+      <c r="B72" s="7">
         <v>1</v>
       </c>
-      <c r="E71" s="6">
-        <v>1</v>
-      </c>
-      <c r="F71" s="6">
+      <c r="C72" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" s="1">
         <v>2</v>
       </c>
-      <c r="G71" s="6">
-        <v>3</v>
-      </c>
-      <c r="H71" s="24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8">
-      <c r="A72" s="19">
-        <v>10000000</v>
-      </c>
-      <c r="B72" s="12">
-        <v>1</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D72" s="2">
+      <c r="E72" s="1">
         <v>2</v>
       </c>
-      <c r="E72" s="2">
-        <v>2</v>
-      </c>
-      <c r="F72" s="2">
-        <v>6</v>
-      </c>
-      <c r="G72" s="2">
+      <c r="F72" s="1">
         <v>9</v>
       </c>
-      <c r="H72" s="20" t="s">
-        <v>8</v>
+      <c r="G72" s="1">
+        <v>9</v>
+      </c>
+      <c r="H72" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" s="21"/>
-      <c r="B73" s="13">
+      <c r="B73" s="8">
         <v>2</v>
       </c>
-      <c r="C73" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D73" s="4">
+      <c r="C73" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" s="3">
         <v>3</v>
       </c>
-      <c r="E73" s="4">
+      <c r="E73" s="3">
         <v>2</v>
       </c>
-      <c r="F73" s="4">
-        <v>5</v>
-      </c>
-      <c r="G73" s="4">
+      <c r="F73" s="3">
+        <v>9</v>
+      </c>
+      <c r="G73" s="3">
         <v>6</v>
       </c>
-      <c r="H73" s="22" t="s">
-        <v>8</v>
+      <c r="H73" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" s="21"/>
-      <c r="B74" s="13">
+      <c r="B74" s="8">
         <v>3</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C74" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" s="3">
+        <v>3</v>
+      </c>
+      <c r="E74" s="3">
+        <v>2</v>
+      </c>
+      <c r="F74" s="3">
         <v>8</v>
       </c>
-      <c r="D74" s="4">
-        <v>3</v>
-      </c>
-      <c r="E74" s="4">
-        <v>2</v>
-      </c>
-      <c r="F74" s="4">
-        <v>5</v>
-      </c>
-      <c r="G74" s="4">
-        <v>7</v>
-      </c>
-      <c r="H74" s="22" t="s">
-        <v>8</v>
+      <c r="G74" s="3">
+        <v>7</v>
+      </c>
+      <c r="H74" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" s="21"/>
-      <c r="B75" s="13">
+      <c r="B75" s="8">
         <v>4</v>
       </c>
-      <c r="C75" s="4" t="s">
+      <c r="C75" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75" s="3">
+        <v>3</v>
+      </c>
+      <c r="E75" s="3">
+        <v>2</v>
+      </c>
+      <c r="F75" s="3">
         <v>8</v>
       </c>
-      <c r="D75" s="4">
+      <c r="G75" s="3">
+        <v>7</v>
+      </c>
+      <c r="H75" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="22"/>
+      <c r="B76" s="9">
+        <v>5</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" s="5">
         <v>3</v>
       </c>
-      <c r="E75" s="4">
+      <c r="E76" s="5">
         <v>2</v>
       </c>
-      <c r="F75" s="4">
-        <v>6</v>
-      </c>
-      <c r="G75" s="4">
-        <v>7</v>
-      </c>
-      <c r="H75" s="22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8">
-      <c r="A76" s="23"/>
-      <c r="B76" s="14">
+      <c r="F76" s="5">
+        <v>9</v>
+      </c>
+      <c r="G76" s="5">
+        <v>7</v>
+      </c>
+      <c r="H76" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="20">
+        <v>20000000</v>
+      </c>
+      <c r="B77" s="7">
+        <v>1</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" s="1">
         <v>5</v>
       </c>
-      <c r="C76" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D76" s="6">
-        <v>3</v>
-      </c>
-      <c r="E76" s="6">
-        <v>2</v>
-      </c>
-      <c r="F76" s="6">
-        <v>6</v>
-      </c>
-      <c r="G76" s="6">
-        <v>7</v>
-      </c>
-      <c r="H76" s="24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8">
-      <c r="A77" s="19">
-        <v>20000000</v>
-      </c>
-      <c r="B77" s="12">
-        <v>1</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D77" s="2">
+      <c r="E77" s="1">
         <v>5</v>
       </c>
-      <c r="E77" s="2">
-        <v>5</v>
-      </c>
-      <c r="F77" s="2">
-        <v>11</v>
-      </c>
-      <c r="G77" s="2">
+      <c r="F77" s="1">
+        <v>18</v>
+      </c>
+      <c r="G77" s="1">
         <v>15</v>
       </c>
-      <c r="H77" s="20" t="s">
-        <v>8</v>
+      <c r="H77" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:8">
       <c r="A78" s="21"/>
-      <c r="B78" s="13">
+      <c r="B78" s="8">
         <v>2</v>
       </c>
-      <c r="C78" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D78" s="4">
+      <c r="C78" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D78" s="3">
         <v>5</v>
       </c>
-      <c r="E78" s="4">
+      <c r="E78" s="3">
         <v>5</v>
       </c>
-      <c r="F78" s="4">
-        <v>12</v>
-      </c>
-      <c r="G78" s="4">
+      <c r="F78" s="3">
+        <v>18</v>
+      </c>
+      <c r="G78" s="3">
         <v>16</v>
       </c>
-      <c r="H78" s="22" t="s">
-        <v>8</v>
+      <c r="H78" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="79" spans="1:8">
       <c r="A79" s="21"/>
-      <c r="B79" s="13">
+      <c r="B79" s="8">
         <v>3</v>
       </c>
-      <c r="C79" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D79" s="4">
+      <c r="C79" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D79" s="3">
         <v>5</v>
       </c>
-      <c r="E79" s="4">
+      <c r="E79" s="3">
         <v>5</v>
       </c>
-      <c r="F79" s="4">
-        <v>11</v>
-      </c>
-      <c r="G79" s="4">
+      <c r="F79" s="3">
+        <v>18</v>
+      </c>
+      <c r="G79" s="3">
         <v>16</v>
       </c>
-      <c r="H79" s="22" t="s">
-        <v>8</v>
+      <c r="H79" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:8">
       <c r="A80" s="21"/>
-      <c r="B80" s="13">
+      <c r="B80" s="8">
         <v>4</v>
       </c>
-      <c r="C80" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D80" s="4">
+      <c r="C80" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D80" s="3">
         <v>6</v>
       </c>
-      <c r="E80" s="4">
+      <c r="E80" s="3">
         <v>5</v>
       </c>
-      <c r="F80" s="4">
-        <v>10</v>
-      </c>
-      <c r="G80" s="4">
+      <c r="F80" s="3">
+        <v>17</v>
+      </c>
+      <c r="G80" s="3">
         <v>15</v>
       </c>
-      <c r="H80" s="22" t="s">
-        <v>8</v>
+      <c r="H80" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="81" spans="1:8">
-      <c r="A81" s="23"/>
-      <c r="B81" s="14">
+      <c r="A81" s="22"/>
+      <c r="B81" s="9">
         <v>5</v>
       </c>
-      <c r="C81" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D81" s="6">
+      <c r="C81" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81" s="5">
         <v>5</v>
       </c>
-      <c r="E81" s="6">
+      <c r="E81" s="5">
         <v>4</v>
       </c>
-      <c r="F81" s="6">
-        <v>10</v>
-      </c>
-      <c r="G81" s="6">
+      <c r="F81" s="5">
+        <v>16</v>
+      </c>
+      <c r="G81" s="5">
         <v>15</v>
       </c>
-      <c r="H81" s="24" t="s">
-        <v>8</v>
+      <c r="H81" s="16" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="82" spans="1:8">
-      <c r="A82" s="19">
+      <c r="A82" s="20">
         <v>50000000</v>
       </c>
-      <c r="B82" s="12">
+      <c r="B82" s="7">
         <v>1</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D82" s="2">
+      <c r="C82" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82" s="1">
         <v>13</v>
       </c>
-      <c r="E82" s="2">
+      <c r="E82" s="1">
         <v>15</v>
       </c>
-      <c r="F82" s="2">
-        <v>29</v>
-      </c>
-      <c r="G82" s="2">
+      <c r="F82" s="1">
         <v>47</v>
       </c>
-      <c r="H82" s="20" t="s">
-        <v>8</v>
+      <c r="G82" s="1">
+        <v>47</v>
+      </c>
+      <c r="H82" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="83" spans="1:8">
       <c r="A83" s="21"/>
-      <c r="B83" s="13">
+      <c r="B83" s="8">
         <v>2</v>
       </c>
-      <c r="C83" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D83" s="4">
+      <c r="C83" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83" s="3">
         <v>14</v>
       </c>
-      <c r="E83" s="4">
+      <c r="E83" s="3">
         <v>13</v>
       </c>
-      <c r="F83" s="4">
-        <v>27</v>
-      </c>
-      <c r="G83" s="4">
+      <c r="F83" s="3">
         <v>46</v>
       </c>
-      <c r="H83" s="22" t="s">
-        <v>8</v>
+      <c r="G83" s="3">
+        <v>46</v>
+      </c>
+      <c r="H83" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="84" spans="1:8">
       <c r="A84" s="21"/>
-      <c r="B84" s="13">
+      <c r="B84" s="8">
         <v>3</v>
       </c>
-      <c r="C84" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D84" s="4">
+      <c r="C84" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D84" s="3">
         <v>13</v>
       </c>
-      <c r="E84" s="4">
+      <c r="E84" s="3">
         <v>13</v>
       </c>
-      <c r="F84" s="4">
-        <v>29</v>
-      </c>
-      <c r="G84" s="4">
+      <c r="F84" s="3">
+        <v>48</v>
+      </c>
+      <c r="G84" s="3">
         <v>51</v>
       </c>
-      <c r="H84" s="22" t="s">
-        <v>8</v>
+      <c r="H84" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="85" spans="1:8">
       <c r="A85" s="21"/>
-      <c r="B85" s="13">
+      <c r="B85" s="8">
         <v>4</v>
       </c>
-      <c r="C85" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D85" s="4">
+      <c r="C85" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85" s="3">
         <v>13</v>
       </c>
-      <c r="E85" s="4">
+      <c r="E85" s="3">
         <v>12</v>
       </c>
-      <c r="F85" s="4">
+      <c r="F85" s="3">
+        <v>49</v>
+      </c>
+      <c r="G85" s="3">
+        <v>47</v>
+      </c>
+      <c r="H85" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" s="22"/>
+      <c r="B86" s="9">
+        <v>5</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D86" s="5">
+        <v>13</v>
+      </c>
+      <c r="E86" s="5">
+        <v>12</v>
+      </c>
+      <c r="F86" s="5">
+        <v>48</v>
+      </c>
+      <c r="G86" s="5">
+        <v>46</v>
+      </c>
+      <c r="H86" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" s="23">
+        <v>100000000</v>
+      </c>
+      <c r="B87" s="7">
+        <v>1</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D87" s="18">
+        <v>31</v>
+      </c>
+      <c r="E87" s="18">
+        <v>30</v>
+      </c>
+      <c r="F87" s="18">
+        <v>92</v>
+      </c>
+      <c r="G87" s="18">
+        <v>112</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88" s="24"/>
+      <c r="B88" s="8">
+        <v>2</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D88" s="17">
+        <v>29</v>
+      </c>
+      <c r="E88" s="17">
+        <v>30</v>
+      </c>
+      <c r="F88" s="17">
+        <v>100</v>
+      </c>
+      <c r="G88" s="17">
+        <v>114</v>
+      </c>
+      <c r="H88" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89" s="24"/>
+      <c r="B89" s="8">
+        <v>3</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D89" s="17">
         <v>28</v>
       </c>
-      <c r="G85" s="4">
-        <v>47</v>
-      </c>
-      <c r="H85" s="22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8">
-      <c r="A86" s="23"/>
-      <c r="B86" s="14">
+      <c r="E89" s="17">
+        <v>25</v>
+      </c>
+      <c r="F89" s="17">
+        <v>98</v>
+      </c>
+      <c r="G89" s="17">
+        <v>115</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" s="24"/>
+      <c r="B90" s="8">
+        <v>4</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D90" s="17">
+        <v>31</v>
+      </c>
+      <c r="E90" s="17">
+        <v>26</v>
+      </c>
+      <c r="F90" s="17">
+        <v>92</v>
+      </c>
+      <c r="G90" s="17">
+        <v>115</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" s="25"/>
+      <c r="B91" s="9">
         <v>5</v>
       </c>
-      <c r="C86" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D86" s="6">
-        <v>13</v>
-      </c>
-      <c r="E86" s="6">
-        <v>12</v>
-      </c>
-      <c r="F86" s="6">
+      <c r="C91" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D91" s="5">
+        <v>30</v>
+      </c>
+      <c r="E91" s="5">
         <v>27</v>
       </c>
-      <c r="G86" s="6">
-        <v>46</v>
-      </c>
-      <c r="H86" s="24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8">
-      <c r="A87" s="10">
-        <v>100000000</v>
-      </c>
-      <c r="B87" s="12">
+      <c r="F91" s="5">
+        <v>97</v>
+      </c>
+      <c r="G91" s="5">
+        <v>115</v>
+      </c>
+      <c r="H91" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="A92" s="23">
+        <v>200000000</v>
+      </c>
+      <c r="B92" s="7">
         <v>1</v>
       </c>
-      <c r="C87" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D87" s="26">
-        <v>31</v>
-      </c>
-      <c r="E87" s="26">
-        <v>30</v>
-      </c>
-      <c r="F87" s="26">
-        <v>61</v>
-      </c>
-      <c r="G87" s="26">
-        <v>112</v>
-      </c>
-      <c r="H87" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8">
-      <c r="A88" s="9"/>
-      <c r="B88" s="13">
+      <c r="C92" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D92" s="1">
+        <v>59</v>
+      </c>
+      <c r="E92" s="1">
+        <v>57</v>
+      </c>
+      <c r="F92" s="1">
+        <v>227</v>
+      </c>
+      <c r="G92" s="1">
+        <v>248</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8">
+      <c r="A93" s="24"/>
+      <c r="B93" s="19">
         <v>2</v>
       </c>
-      <c r="C88" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D88" s="25">
-        <v>29</v>
-      </c>
-      <c r="E88" s="25">
-        <v>30</v>
-      </c>
-      <c r="F88" s="25">
-        <v>60</v>
-      </c>
-      <c r="G88" s="25">
-        <v>114</v>
-      </c>
-      <c r="H88" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8">
-      <c r="A89" s="9"/>
-      <c r="B89" s="13">
+      <c r="C93" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D93" s="17">
+        <v>56</v>
+      </c>
+      <c r="E93" s="17">
+        <v>57</v>
+      </c>
+      <c r="F93" s="17">
+        <v>231</v>
+      </c>
+      <c r="G93" s="17">
+        <v>237</v>
+      </c>
+      <c r="H93" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="A94" s="24"/>
+      <c r="B94" s="19">
         <v>3</v>
       </c>
-      <c r="C89" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D89" s="25">
-        <v>28</v>
-      </c>
-      <c r="E89" s="25">
-        <v>25</v>
-      </c>
-      <c r="F89" s="25">
+      <c r="C94" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D94" s="17">
+        <v>57</v>
+      </c>
+      <c r="E94" s="17">
+        <v>56</v>
+      </c>
+      <c r="F94" s="17">
+        <v>243</v>
+      </c>
+      <c r="G94" s="17">
+        <v>252</v>
+      </c>
+      <c r="H94" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8">
+      <c r="A95" s="24"/>
+      <c r="B95" s="19">
+        <v>4</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D95" s="17">
+        <v>57</v>
+      </c>
+      <c r="E95" s="17">
+        <v>55</v>
+      </c>
+      <c r="F95" s="17">
+        <v>217</v>
+      </c>
+      <c r="G95" s="17">
+        <v>237</v>
+      </c>
+      <c r="H95" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
+      <c r="A96" s="25"/>
+      <c r="B96" s="9">
+        <v>5</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D96" s="5">
+        <v>62</v>
+      </c>
+      <c r="E96" s="5">
         <v>58</v>
       </c>
-      <c r="G89" s="25">
-        <v>115</v>
-      </c>
-      <c r="H89" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8">
-      <c r="A90" s="9"/>
-      <c r="B90" s="13">
-        <v>4</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D90" s="25">
-        <v>31</v>
-      </c>
-      <c r="E90" s="25">
-        <v>26</v>
-      </c>
-      <c r="F90" s="25">
-        <v>62</v>
-      </c>
-      <c r="G90" s="25">
-        <v>115</v>
-      </c>
-      <c r="H90" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8">
-      <c r="A91" s="11"/>
-      <c r="B91" s="14">
-        <v>5</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D91" s="6">
-        <v>30</v>
-      </c>
-      <c r="E91" s="6">
-        <v>27</v>
-      </c>
-      <c r="F91" s="6">
-        <v>57</v>
-      </c>
-      <c r="G91" s="6">
-        <v>115</v>
-      </c>
-      <c r="H91" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8">
-      <c r="A92" s="10">
-        <v>200000000</v>
-      </c>
-      <c r="B92" s="12">
-        <v>1</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D92" s="2">
-        <v>59</v>
-      </c>
-      <c r="E92" s="2">
-        <v>57</v>
-      </c>
-      <c r="F92" s="2">
-        <v>125</v>
-      </c>
-      <c r="G92" s="2">
-        <v>248</v>
-      </c>
-      <c r="H92" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8">
-      <c r="A93" s="9"/>
-      <c r="B93" s="27">
-        <v>2</v>
-      </c>
-      <c r="C93" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D93" s="25">
-        <v>56</v>
-      </c>
-      <c r="E93" s="25">
-        <v>57</v>
-      </c>
-      <c r="F93" s="25">
-        <v>117</v>
-      </c>
-      <c r="G93" s="25">
-        <v>237</v>
-      </c>
-      <c r="H93" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8">
-      <c r="A94" s="9"/>
-      <c r="B94" s="27">
-        <v>3</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D94" s="25">
-        <v>57</v>
-      </c>
-      <c r="E94" s="25">
-        <v>56</v>
-      </c>
-      <c r="F94" s="25">
-        <v>126</v>
-      </c>
-      <c r="G94" s="25">
-        <v>252</v>
-      </c>
-      <c r="H94" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8">
-      <c r="A95" s="9"/>
-      <c r="B95" s="27">
-        <v>4</v>
-      </c>
-      <c r="C95" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D95" s="25">
-        <v>57</v>
-      </c>
-      <c r="E95" s="25">
-        <v>55</v>
-      </c>
-      <c r="F95" s="25">
-        <v>123</v>
-      </c>
-      <c r="G95" s="25">
-        <v>237</v>
-      </c>
-      <c r="H95" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8">
-      <c r="A96" s="11"/>
-      <c r="B96" s="14">
-        <v>5</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D96" s="6">
-        <v>62</v>
-      </c>
-      <c r="E96" s="6">
-        <v>58</v>
-      </c>
-      <c r="F96" s="6">
-        <v>119</v>
-      </c>
-      <c r="G96" s="6">
+      <c r="F96" s="5">
+        <v>212</v>
+      </c>
+      <c r="G96" s="5">
         <v>261</v>
       </c>
-      <c r="H96" s="7" t="s">
-        <v>8</v>
+      <c r="H96" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97" s="8"/>
+      <c r="A97" s="26"/>
     </row>
     <row r="98" spans="1:1">
-      <c r="A98" s="1"/>
+      <c r="A98" s="27"/>
     </row>
     <row r="99" spans="1:1">
-      <c r="A99" s="1"/>
+      <c r="A99" s="27"/>
     </row>
     <row r="100" spans="1:1">
-      <c r="A100" s="1"/>
+      <c r="A100" s="27"/>
     </row>
     <row r="101" spans="1:1">
-      <c r="A101" s="1"/>
+      <c r="A101" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -6298,11 +6282,6 @@
     <mergeCell ref="A77:A81"/>
     <mergeCell ref="A82:A86"/>
     <mergeCell ref="A87:A91"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="A47:A51"/>
-    <mergeCell ref="A52:A56"/>
     <mergeCell ref="A57:A61"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A11"/>
@@ -6310,6 +6289,11 @@
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="A52:A56"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6320,9 +6304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD8D8BCE-0BDE-3842-A799-246FA9923D66}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <sheetData>
@@ -6337,16 +6319,16 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -6641,7 +6623,7 @@
       </c>
       <c r="E12">
         <f>AVERAGE(Data!F52:F56)</f>
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="F12">
         <f>AVERAGE(Data!G52:G56)</f>
@@ -6683,7 +6665,7 @@
       </c>
       <c r="E14">
         <f>AVERAGE(Data!F62:F66)</f>
-        <v>0.8</v>
+        <v>1.8</v>
       </c>
       <c r="F14">
         <f>AVERAGE(Data!G62:G66)</f>
@@ -6704,7 +6686,7 @@
       </c>
       <c r="E15">
         <f>AVERAGE(Data!F67:F71)</f>
-        <v>2.4</v>
+        <v>4</v>
       </c>
       <c r="F15">
         <f>AVERAGE(Data!G67:G71)</f>
@@ -6725,7 +6707,7 @@
       </c>
       <c r="E16">
         <f>AVERAGE(Data!F72:F76)</f>
-        <v>5.6</v>
+        <v>8.6</v>
       </c>
       <c r="F16">
         <f>AVERAGE(Data!G72:G76)</f>
@@ -6746,7 +6728,7 @@
       </c>
       <c r="E17">
         <f>AVERAGE(Data!F77:F81)</f>
-        <v>10.8</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="F17">
         <f>AVERAGE(Data!G77:G81)</f>
@@ -6767,7 +6749,7 @@
       </c>
       <c r="E18">
         <f>AVERAGE(Data!F82:F86)</f>
-        <v>28</v>
+        <v>47.6</v>
       </c>
       <c r="F18">
         <f>AVERAGE(Data!G82:G86)</f>
@@ -6788,7 +6770,7 @@
       </c>
       <c r="E19">
         <f>AVERAGE(Data!F87:F91)</f>
-        <v>59.6</v>
+        <v>95.8</v>
       </c>
       <c r="F19">
         <f>AVERAGE(Data!G87:G91)</f>
@@ -6809,7 +6791,7 @@
       </c>
       <c r="E20">
         <f>AVERAGE(Data!F92:F96)</f>
-        <v>122</v>
+        <v>226</v>
       </c>
       <c r="F20">
         <f>AVERAGE(Data!G92:G96)</f>
@@ -6827,7 +6809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8035CBA9-1FCE-9547-8832-5B32A18D26EC}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
@@ -6837,16 +6819,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4">

</xml_diff>